<commit_message>
test data from excel
</commit_message>
<xml_diff>
--- a/assets/test/JLPTN5VocabularyExercise01.xlsx
+++ b/assets/test/JLPTN5VocabularyExercise01.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SAINKHISHIGARIUNAA\Documents\AMJILT\projects\hub\japanese-practice\assets\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364022D0-D21B-4678-AF31-165CC012017B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03DEB1D7-D599-43E5-8D51-5FDE80D92486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6030" yWindow="795" windowWidth="21600" windowHeight="11385" xr2:uid="{420E8C55-19C0-40C9-A56F-FFAB79D10407}"/>
+    <workbookView xWindow="6030" yWindow="795" windowWidth="14025" windowHeight="9975" xr2:uid="{420E8C55-19C0-40C9-A56F-FFAB79D10407}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -552,7 +553,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -764,4 +765,22 @@
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09063DCF-DDD7-4AE9-BD85-7AFC4A4FB0F5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="9" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>